<commit_message>
search box and search button have been added. Pwede na rin po magsearch mula sa excel file.
</commit_message>
<xml_diff>
--- a/Contact Tracing Data.xlsx
+++ b/Contact Tracing Data.xlsx
@@ -412,10 +412,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="I4" sqref="A2:I4"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -425,9 +425,9 @@
     <col width="27" customWidth="1" min="3" max="3"/>
     <col width="25.6640625" customWidth="1" min="4" max="4"/>
     <col width="39.33203125" customWidth="1" min="5" max="5"/>
-    <col width="10.109375" customWidth="1" min="6" max="6"/>
+    <col width="12.6640625" customWidth="1" min="6" max="6"/>
     <col width="15.21875" customWidth="1" min="7" max="7"/>
-    <col width="15.5546875" customWidth="1" min="8" max="8"/>
+    <col width="21.109375" customWidth="1" min="8" max="8"/>
     <col width="59.33203125" customWidth="1" min="9" max="9"/>
   </cols>
   <sheetData>
@@ -481,12 +481,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>mary grace</t>
+          <t>Mary Grace</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>dellomos</t>
+          <t>Dellomos</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -501,74 +501,27 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Tanza, Cavite</t>
+          <t>etivac</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>6:30 A.M.</t>
+          <t>4:50 A.M.</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>2023</t>
+          <t>26/07/2023</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Second Booster Shot</t>
+          <t>First Booster Shot</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>No, Sore Throat, Loss of Taste and Smell, Muscles and Body Pains</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>mary grace</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>dellomos</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>0988</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>meji@gmail.com</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Tanza, Cavite</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>6:30 A.M.</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>2023</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Second Booster Shot</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>No, Sore Throat, Loss of Taste and Smell, Muscles and Body Pains</t>
+          <t>No, Fever, Cough</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
a scrollable frame for the searched data to displayed has been added
</commit_message>
<xml_diff>
--- a/Contact Tracing Data.xlsx
+++ b/Contact Tracing Data.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
@@ -525,6 +525,194 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>lolo</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>dellomos</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>manila</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>6:15 A.M.</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>26/07/2023</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>No, Fever, Cough</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>kate</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>dellomos</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>26/07/2023</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>First Dose</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Fever</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>jade</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>dellomos</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>09</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>s</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Second Dose</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Sore Throat</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>dellomos</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>m</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>First Booster Shot</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Fever</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
code has been modified
</commit_message>
<xml_diff>
--- a/Contact Tracing Data.xlsx
+++ b/Contact Tracing Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mary Grace\Desktop\Object-Oriented Programming\FinalProject-Contact-Tracing-App-GUI\FinalProject-Contact-Tracing-App-GUI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9CC8299-CD37-4DC3-A8F8-CCFDB0A6D1C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEF64DF-C0F9-4D2D-B00C-E83E17BFA771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1920" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,21 +388,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="I4" sqref="A2:I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" customWidth="1"/>
-    <col min="2" max="2" width="28.33203125" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="39.33203125" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.21875" customWidth="1"/>
-    <col min="8" max="8" width="21.109375" customWidth="1"/>
-    <col min="9" max="9" width="59.33203125" customWidth="1"/>
+    <col min="1" max="1" width="26.6640625" customWidth="1"/>
+    <col min="2" max="2" width="26.77734375" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="26.77734375" customWidth="1"/>
+    <col min="5" max="5" width="44.77734375" customWidth="1"/>
+    <col min="6" max="6" width="11.77734375" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="53.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">

</xml_diff>